<commit_message>
reruns after data source adjustments
</commit_message>
<xml_diff>
--- a/Vjerojatnost smrti populacije od kriticnih bolesti i zdravih od ostalih bolesti_gamma_0,25.xlsx
+++ b/Vjerojatnost smrti populacije od kriticnih bolesti i zdravih od ostalih bolesti_gamma_0,25.xlsx
@@ -354,7 +354,7 @@
   <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -386,13 +386,13 @@
         <v>20</v>
       </c>
       <c r="B2">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C2">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D2">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E2">
         <v>9.31498E-4</v>
@@ -403,13 +403,13 @@
         <v>21</v>
       </c>
       <c r="B3">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C3">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D3">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E3">
         <v>9.31498E-4</v>
@@ -420,13 +420,13 @@
         <v>22</v>
       </c>
       <c r="B4">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C4">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D4">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E4">
         <v>9.31498E-4</v>
@@ -437,13 +437,13 @@
         <v>23</v>
       </c>
       <c r="B5">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C5">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D5">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E5">
         <v>9.31498E-4</v>
@@ -454,13 +454,13 @@
         <v>24</v>
       </c>
       <c r="B6">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C6">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D6">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E6">
         <v>9.31498E-4</v>
@@ -471,13 +471,13 @@
         <v>25</v>
       </c>
       <c r="B7">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C7">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D7">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E7">
         <v>9.31498E-4</v>
@@ -488,13 +488,13 @@
         <v>26</v>
       </c>
       <c r="B8">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C8">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D8">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E8">
         <v>9.31498E-4</v>
@@ -505,13 +505,13 @@
         <v>27</v>
       </c>
       <c r="B9">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C9">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D9">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E9">
         <v>9.31498E-4</v>
@@ -522,13 +522,13 @@
         <v>28</v>
       </c>
       <c r="B10">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C10">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D10">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E10">
         <v>9.31498E-4</v>
@@ -539,13 +539,13 @@
         <v>29</v>
       </c>
       <c r="B11">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C11">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D11">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E11">
         <v>9.31498E-4</v>
@@ -556,13 +556,13 @@
         <v>30</v>
       </c>
       <c r="B12">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C12">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D12">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E12">
         <v>9.31498E-4</v>
@@ -573,13 +573,13 @@
         <v>31</v>
       </c>
       <c r="B13">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C13">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D13">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E13">
         <v>9.31498E-4</v>
@@ -590,13 +590,13 @@
         <v>32</v>
       </c>
       <c r="B14">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C14">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D14">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E14">
         <v>9.31498E-4</v>
@@ -607,13 +607,13 @@
         <v>33</v>
       </c>
       <c r="B15">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C15">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D15">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E15">
         <v>9.31498E-4</v>
@@ -624,13 +624,13 @@
         <v>34</v>
       </c>
       <c r="B16">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C16">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D16">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E16">
         <v>9.31498E-4</v>
@@ -641,13 +641,13 @@
         <v>35</v>
       </c>
       <c r="B17">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C17">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D17">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E17">
         <v>9.31498E-4</v>
@@ -658,13 +658,13 @@
         <v>36</v>
       </c>
       <c r="B18">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C18">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D18">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E18">
         <v>9.31498E-4</v>
@@ -675,13 +675,13 @@
         <v>37</v>
       </c>
       <c r="B19">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C19">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D19">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E19">
         <v>9.31498E-4</v>
@@ -692,13 +692,13 @@
         <v>38</v>
       </c>
       <c r="B20">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C20">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D20">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E20">
         <v>9.31498E-4</v>
@@ -709,13 +709,13 @@
         <v>39</v>
       </c>
       <c r="B21">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C21">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D21">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E21">
         <v>9.31498E-4</v>
@@ -726,13 +726,13 @@
         <v>40</v>
       </c>
       <c r="B22">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C22">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D22">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E22">
         <v>9.31498E-4</v>
@@ -743,13 +743,13 @@
         <v>41</v>
       </c>
       <c r="B23">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C23">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D23">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E23">
         <v>9.31498E-4</v>
@@ -760,13 +760,13 @@
         <v>42</v>
       </c>
       <c r="B24">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C24">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D24">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E24">
         <v>9.31498E-4</v>
@@ -777,13 +777,13 @@
         <v>43</v>
       </c>
       <c r="B25">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C25">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D25">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E25">
         <v>9.31498E-4</v>
@@ -794,13 +794,13 @@
         <v>44</v>
       </c>
       <c r="B26">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C26">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D26">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E26">
         <v>9.31498E-4</v>
@@ -811,13 +811,13 @@
         <v>45</v>
       </c>
       <c r="B27">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C27">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D27">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E27">
         <v>9.31498E-4</v>
@@ -828,13 +828,13 @@
         <v>46</v>
       </c>
       <c r="B28">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C28">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D28">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E28">
         <v>9.31498E-4</v>
@@ -845,13 +845,13 @@
         <v>47</v>
       </c>
       <c r="B29">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C29">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D29">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E29">
         <v>9.31498E-4</v>
@@ -862,13 +862,13 @@
         <v>48</v>
       </c>
       <c r="B30">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C30">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D30">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E30">
         <v>9.31498E-4</v>
@@ -879,13 +879,13 @@
         <v>49</v>
       </c>
       <c r="B31">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C31">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D31">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E31">
         <v>9.31498E-4</v>
@@ -896,13 +896,13 @@
         <v>50</v>
       </c>
       <c r="B32">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C32">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D32">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E32">
         <v>9.31498E-4</v>
@@ -913,13 +913,13 @@
         <v>51</v>
       </c>
       <c r="B33">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C33">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D33">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E33">
         <v>9.31498E-4</v>
@@ -930,13 +930,13 @@
         <v>52</v>
       </c>
       <c r="B34">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C34">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D34">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E34">
         <v>9.31498E-4</v>
@@ -947,13 +947,13 @@
         <v>53</v>
       </c>
       <c r="B35">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C35">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D35">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E35">
         <v>9.31498E-4</v>
@@ -964,13 +964,13 @@
         <v>54</v>
       </c>
       <c r="B36">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C36">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D36">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E36">
         <v>9.31498E-4</v>
@@ -981,13 +981,13 @@
         <v>55</v>
       </c>
       <c r="B37">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C37">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D37">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E37">
         <v>9.31498E-4</v>
@@ -998,13 +998,13 @@
         <v>56</v>
       </c>
       <c r="B38">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C38">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D38">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E38">
         <v>9.31498E-4</v>
@@ -1015,13 +1015,13 @@
         <v>57</v>
       </c>
       <c r="B39">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C39">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D39">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E39">
         <v>9.31498E-4</v>
@@ -1032,13 +1032,13 @@
         <v>58</v>
       </c>
       <c r="B40">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C40">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D40">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E40">
         <v>9.31498E-4</v>
@@ -1049,13 +1049,13 @@
         <v>59</v>
       </c>
       <c r="B41">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C41">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D41">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E41">
         <v>9.31498E-4</v>
@@ -1066,13 +1066,13 @@
         <v>60</v>
       </c>
       <c r="B42">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C42">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D42">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E42">
         <v>9.31498E-4</v>
@@ -1083,13 +1083,13 @@
         <v>61</v>
       </c>
       <c r="B43">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C43">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D43">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E43">
         <v>9.31498E-4</v>
@@ -1100,13 +1100,13 @@
         <v>62</v>
       </c>
       <c r="B44">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C44">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D44">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E44">
         <v>9.31498E-4</v>
@@ -1117,13 +1117,13 @@
         <v>63</v>
       </c>
       <c r="B45">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C45">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D45">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E45">
         <v>9.31498E-4</v>
@@ -1134,13 +1134,13 @@
         <v>64</v>
       </c>
       <c r="B46">
-        <v>2.0599999999999999E-4</v>
+        <v>4.17E-4</v>
       </c>
       <c r="C46">
-        <v>3.77E-4</v>
+        <v>8.0500000000000005E-4</v>
       </c>
       <c r="D46">
-        <v>8.0400000000000003E-4</v>
+        <v>1.5269999999999999E-3</v>
       </c>
       <c r="E46">
         <v>9.31498E-4</v>
@@ -1151,13 +1151,13 @@
         <v>65</v>
       </c>
       <c r="B47">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C47">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D47">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E47">
         <v>7.7724719999999999E-3</v>
@@ -1168,13 +1168,13 @@
         <v>66</v>
       </c>
       <c r="B48">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C48">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D48">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E48">
         <v>7.7724719999999999E-3</v>
@@ -1185,13 +1185,13 @@
         <v>67</v>
       </c>
       <c r="B49">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C49">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D49">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E49">
         <v>7.7724719999999999E-3</v>
@@ -1202,13 +1202,13 @@
         <v>68</v>
       </c>
       <c r="B50">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C50">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D50">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E50">
         <v>7.7724719999999999E-3</v>
@@ -1219,13 +1219,13 @@
         <v>69</v>
       </c>
       <c r="B51">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C51">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D51">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E51">
         <v>7.7724719999999999E-3</v>
@@ -1236,13 +1236,13 @@
         <v>70</v>
       </c>
       <c r="B52">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C52">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D52">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E52">
         <v>7.7724719999999999E-3</v>
@@ -1253,13 +1253,13 @@
         <v>71</v>
       </c>
       <c r="B53">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C53">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D53">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E53">
         <v>7.7724719999999999E-3</v>
@@ -1270,13 +1270,13 @@
         <v>72</v>
       </c>
       <c r="B54">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C54">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D54">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E54">
         <v>7.7724719999999999E-3</v>
@@ -1287,13 +1287,13 @@
         <v>73</v>
       </c>
       <c r="B55">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C55">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D55">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E55">
         <v>7.7724719999999999E-3</v>
@@ -1304,13 +1304,13 @@
         <v>74</v>
       </c>
       <c r="B56">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C56">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D56">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E56">
         <v>7.7724719999999999E-3</v>
@@ -1321,13 +1321,13 @@
         <v>75</v>
       </c>
       <c r="B57">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C57">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D57">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E57">
         <v>7.7724719999999999E-3</v>
@@ -1338,13 +1338,13 @@
         <v>76</v>
       </c>
       <c r="B58">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C58">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D58">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E58">
         <v>7.7724719999999999E-3</v>
@@ -1355,13 +1355,13 @@
         <v>77</v>
       </c>
       <c r="B59">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C59">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D59">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E59">
         <v>7.7724719999999999E-3</v>
@@ -1372,13 +1372,13 @@
         <v>78</v>
       </c>
       <c r="B60">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C60">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D60">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E60">
         <v>7.7724719999999999E-3</v>
@@ -1389,13 +1389,13 @@
         <v>79</v>
       </c>
       <c r="B61">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C61">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D61">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E61">
         <v>7.7724719999999999E-3</v>
@@ -1406,13 +1406,13 @@
         <v>80</v>
       </c>
       <c r="B62">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C62">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D62">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E62">
         <v>7.7724719999999999E-3</v>
@@ -1423,13 +1423,13 @@
         <v>81</v>
       </c>
       <c r="B63">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C63">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D63">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E63">
         <v>7.7724719999999999E-3</v>
@@ -1440,13 +1440,13 @@
         <v>82</v>
       </c>
       <c r="B64">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C64">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D64">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E64">
         <v>7.7724719999999999E-3</v>
@@ -1457,13 +1457,13 @@
         <v>83</v>
       </c>
       <c r="B65">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C65">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D65">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E65">
         <v>7.7724719999999999E-3</v>
@@ -1474,13 +1474,13 @@
         <v>84</v>
       </c>
       <c r="B66">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C66">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D66">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E66">
         <v>7.7724719999999999E-3</v>
@@ -1491,13 +1491,13 @@
         <v>85</v>
       </c>
       <c r="B67">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C67">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D67">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E67">
         <v>7.7724719999999999E-3</v>
@@ -1508,13 +1508,13 @@
         <v>86</v>
       </c>
       <c r="B68">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C68">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D68">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E68">
         <v>7.7724719999999999E-3</v>
@@ -1525,13 +1525,13 @@
         <v>87</v>
       </c>
       <c r="B69">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C69">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D69">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E69">
         <v>7.7724719999999999E-3</v>
@@ -1542,13 +1542,13 @@
         <v>88</v>
       </c>
       <c r="B70">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C70">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D70">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E70">
         <v>7.7724719999999999E-3</v>
@@ -1559,13 +1559,13 @@
         <v>89</v>
       </c>
       <c r="B71">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C71">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D71">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E71">
         <v>7.7724719999999999E-3</v>
@@ -1576,13 +1576,13 @@
         <v>90</v>
       </c>
       <c r="B72">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C72">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D72">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E72">
         <v>7.7724719999999999E-3</v>
@@ -1593,13 +1593,13 @@
         <v>91</v>
       </c>
       <c r="B73">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C73">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D73">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E73">
         <v>7.7724719999999999E-3</v>
@@ -1610,13 +1610,13 @@
         <v>92</v>
       </c>
       <c r="B74">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C74">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D74">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E74">
         <v>7.7724719999999999E-3</v>
@@ -1627,13 +1627,13 @@
         <v>93</v>
       </c>
       <c r="B75">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C75">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D75">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E75">
         <v>7.7724719999999999E-3</v>
@@ -1644,13 +1644,13 @@
         <v>94</v>
       </c>
       <c r="B76">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C76">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D76">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E76">
         <v>7.7724719999999999E-3</v>
@@ -1661,13 +1661,13 @@
         <v>95</v>
       </c>
       <c r="B77">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C77">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D77">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E77">
         <v>7.7724719999999999E-3</v>
@@ -1678,13 +1678,13 @@
         <v>96</v>
       </c>
       <c r="B78">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C78">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D78">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E78">
         <v>7.7724719999999999E-3</v>
@@ -1695,13 +1695,13 @@
         <v>97</v>
       </c>
       <c r="B79">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C79">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D79">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E79">
         <v>7.7724719999999999E-3</v>
@@ -1712,13 +1712,13 @@
         <v>98</v>
       </c>
       <c r="B80">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C80">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D80">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E80">
         <v>7.7724719999999999E-3</v>
@@ -1729,13 +1729,13 @@
         <v>99</v>
       </c>
       <c r="B81">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C81">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D81">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E81">
         <v>7.7724719999999999E-3</v>
@@ -1746,13 +1746,13 @@
         <v>100</v>
       </c>
       <c r="B82">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C82">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D82">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E82">
         <v>7.7724719999999999E-3</v>
@@ -1763,13 +1763,13 @@
         <v>101</v>
       </c>
       <c r="B83">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C83">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D83">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E83">
         <v>7.7724719999999999E-3</v>
@@ -1780,13 +1780,13 @@
         <v>102</v>
       </c>
       <c r="B84">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C84">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D84">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E84">
         <v>7.7724719999999999E-3</v>
@@ -1797,13 +1797,13 @@
         <v>103</v>
       </c>
       <c r="B85">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C85">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D85">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E85">
         <v>7.7724719999999999E-3</v>
@@ -1814,13 +1814,13 @@
         <v>104</v>
       </c>
       <c r="B86">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C86">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D86">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E86">
         <v>7.7724719999999999E-3</v>
@@ -1831,13 +1831,13 @@
         <v>105</v>
       </c>
       <c r="B87">
-        <v>3.7499999999999999E-3</v>
+        <v>5.8129999999999996E-3</v>
       </c>
       <c r="C87">
-        <v>6.862E-3</v>
+        <v>1.1223E-2</v>
       </c>
       <c r="D87">
-        <v>1.4618000000000001E-2</v>
+        <v>2.1295999999999999E-2</v>
       </c>
       <c r="E87">
         <v>7.7724719999999999E-3</v>

</xml_diff>